<commit_message>
Initial parity plot for SciAv
Manually made the sciav_overpasses file because it was too much of a pain to code for so few data points
</commit_message>
<xml_diff>
--- a/00_raw_reports/SciAv_Stage1_submitted-2023-02-21.xlsx
+++ b/00_raw_reports/SciAv_Stage1_submitted-2023-02-21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/00_raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/00_raw_reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43664A62-C3DE-6D4D-A3F9-92953E0900BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AD624D-3CC9-8D40-BE6B-3655AB409177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37300" yWindow="2220" windowWidth="29040" windowHeight="15840" xr2:uid="{AC3A3917-1DB8-476E-8C07-EEBD570C7043}"/>
+    <workbookView xWindow="35020" yWindow="500" windowWidth="21420" windowHeight="19540" xr2:uid="{AC3A3917-1DB8-476E-8C07-EEBD570C7043}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Table" sheetId="12" r:id="rId1"/>
@@ -597,7 +597,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1231,17 +1231,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d753306e-285a-44c6-8280-85ac401334a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fc353d8b-3dd1-4c08-8d95-c533a13405a8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF4A7E0C1C09E0408DE2334E76E485FD" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c0b9d783383bc6aafecc7f20faaede2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d753306e-285a-44c6-8280-85ac401334a2" xmlns:ns3="fc353d8b-3dd1-4c08-8d95-c533a13405a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="31f00eeba95c506051609f8103a99647" ns2:_="" ns3:_="">
     <xsd:import namespace="d753306e-285a-44c6-8280-85ac401334a2"/>
@@ -1484,6 +1473,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d753306e-285a-44c6-8280-85ac401334a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fc353d8b-3dd1-4c08-8d95-c533a13405a8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1494,23 +1494,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E41E6AA-2334-497B-8624-E455A3B4F725}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="d753306e-285a-44c6-8280-85ac401334a2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fc353d8b-3dd1-4c08-8d95-c533a13405a8"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D40DFC-9657-4687-8074-E99047F72E77}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1529,6 +1512,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E41E6AA-2334-497B-8624-E455A3B4F725}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="d753306e-285a-44c6-8280-85ac401334a2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fc353d8b-3dd1-4c08-8d95-c533a13405a8"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8368B9D-8C4E-4762-9B15-D62B6087258A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Revisions to paper figures and analysis based on Evan's feedback
</commit_message>
<xml_diff>
--- a/00_raw_reports/SciAv_Stage1_submitted-2023-02-21.xlsx
+++ b/00_raw_reports/SciAv_Stage1_submitted-2023-02-21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/00_raw_reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AD624D-3CC9-8D40-BE6B-3655AB409177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62D435F-9B22-154F-9407-7D36E2540F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35020" yWindow="500" windowWidth="21420" windowHeight="19540" xr2:uid="{AC3A3917-1DB8-476E-8C07-EEBD570C7043}"/>
+    <workbookView xWindow="39160" yWindow="500" windowWidth="30940" windowHeight="19540" xr2:uid="{AC3A3917-1DB8-476E-8C07-EEBD570C7043}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Table" sheetId="12" r:id="rId1"/>
@@ -597,7 +597,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1231,6 +1231,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d753306e-285a-44c6-8280-85ac401334a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fc353d8b-3dd1-4c08-8d95-c533a13405a8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF4A7E0C1C09E0408DE2334E76E485FD" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c0b9d783383bc6aafecc7f20faaede2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d753306e-285a-44c6-8280-85ac401334a2" xmlns:ns3="fc353d8b-3dd1-4c08-8d95-c533a13405a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="31f00eeba95c506051609f8103a99647" ns2:_="" ns3:_="">
     <xsd:import namespace="d753306e-285a-44c6-8280-85ac401334a2"/>
@@ -1473,17 +1484,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d753306e-285a-44c6-8280-85ac401334a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fc353d8b-3dd1-4c08-8d95-c533a13405a8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1494,6 +1494,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E41E6AA-2334-497B-8624-E455A3B4F725}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="d753306e-285a-44c6-8280-85ac401334a2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fc353d8b-3dd1-4c08-8d95-c533a13405a8"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D40DFC-9657-4687-8074-E99047F72E77}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1512,23 +1529,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E41E6AA-2334-497B-8624-E455A3B4F725}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="d753306e-285a-44c6-8280-85ac401334a2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fc353d8b-3dd1-4c08-8d95-c533a13405a8"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8368B9D-8C4E-4762-9B15-D62B6087258A}">
   <ds:schemaRefs>

</xml_diff>